<commit_message>
Pipedrive and zapier how-tos fixes and updates
</commit_message>
<xml_diff>
--- a/source/_static/files/user-guide/processes/create-xlsx-from-template.xlsx
+++ b/source/_static/files/user-guide/processes/create-xlsx-from-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE25A01E-5AD3-45D7-8216-D786761D1F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533AAD5F-F8C0-4EC6-8E9D-645653725CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>Plumsail LLC</t>
   </si>
   <si>
-    <t>Date: {{Order.Date}}</t>
-  </si>
-  <si>
-    <t>PO: #{{Order.Number}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">3 Main St.New York NY 97203 USA </t>
   </si>
   <si>
@@ -60,36 +54,12 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>{{Vendor.CompanyName}}</t>
-  </si>
-  <si>
-    <t>{{Vendor.Address}}</t>
-  </si>
-  <si>
-    <t>{{Vendor.Phone}}</t>
-  </si>
-  <si>
     <t>Ship To</t>
   </si>
   <si>
-    <t>{{ShipTo.CompanyName}}</t>
-  </si>
-  <si>
-    <t>{{ShipTo.Address}}</t>
-  </si>
-  <si>
-    <t>{{ShipTo.Phone}}</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
-    <t>{{Vendor.Email}}</t>
-  </si>
-  <si>
-    <t>{{ShipTo.Email}}</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -100,6 +70,36 @@
   </si>
   <si>
     <t>{{product.price}}</t>
+  </si>
+  <si>
+    <t>Date: {{orderDate}}</t>
+  </si>
+  <si>
+    <t>PO: #{{orderNumber}}</t>
+  </si>
+  <si>
+    <t>{{vendorName}}</t>
+  </si>
+  <si>
+    <t>{{vendorAddress}}</t>
+  </si>
+  <si>
+    <t>{{vendorEmail}}</t>
+  </si>
+  <si>
+    <t>{{vendorPhone}}</t>
+  </si>
+  <si>
+    <t>{{customerName}}</t>
+  </si>
+  <si>
+    <t>{{customerAddress}}</t>
+  </si>
+  <si>
+    <t>{{customerEmail}}</t>
+  </si>
+  <si>
+    <t>{{customerPhone}}</t>
   </si>
 </sst>
 </file>
@@ -235,25 +235,25 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,94 +646,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="9"/>
+      <c r="A6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -746,18 +746,18 @@
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5" t="e">
         <f>ItemsTable[Quantity]*ItemsTable[Unit Price]</f>
@@ -767,7 +767,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D16" s="7" t="e">
         <f>SUM(D14)</f>
@@ -776,12 +776,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
@@ -792,6 +786,12 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -951,18 +951,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -984,18 +984,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E966EE4D-2DE7-47F5-86C6-BEE999675335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6D7823-0E2C-41FF-AA1E-EEE97275A5B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E966EE4D-2DE7-47F5-86C6-BEE999675335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>